<commit_message>
Adding new TestScript "CreateCustomerWithDEScp"
</commit_message>
<xml_diff>
--- a/actiTimeAutomationProject/data/TestData1.xlsx
+++ b/actiTimeAutomationProject/data/TestData1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10680" windowHeight="2140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12830" windowHeight="3000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>PROJECT_NAME</t>
   </si>
@@ -59,16 +59,28 @@
     <t>p010</t>
   </si>
   <si>
-    <t>AXIS</t>
-  </si>
-  <si>
     <t>AIRTEL</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>HDFC65</t>
+    <t>HDFC659df</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Banglore</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Jaipur</t>
+  </si>
+  <si>
+    <t>AXIS01</t>
   </si>
 </sst>
 </file>
@@ -393,13 +405,14 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="16.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="8.7265625" style="2" collapsed="1"/>
+    <col min="3" max="3" width="15" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -409,17 +422,23 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D2"/>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -427,7 +446,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -435,7 +457,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>